<commit_message>
classificado os 150 primeiros twites
</commit_message>
<xml_diff>
--- a/La casa de papel.xlsx
+++ b/La casa de papel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arthu\Desktop\Documentos\Insper\2º_Periodo\Ciencia_dos_dados\twitter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08DCFE60-A473-4D83-9D94-550BBD8DD113}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C760909D-10D5-41F3-9DA7-E7BC2AA3B2A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2018,8 +2018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B301"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A118" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B151" sqref="B151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2040,793 +2040,1243 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B103">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B104">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B105">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B106">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B111">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B112">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B120">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B121">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B122">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B123">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B124">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B125">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B126">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B127">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B131">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B132">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B133">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B134">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B135">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B136">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B137">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B138">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B139">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B140">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B141">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B142">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B143">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B144">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B145">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B146">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B147">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B148">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B149">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B150">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B151">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>159</v>
       </c>

</xml_diff>

<commit_message>
reclassificando os tweets, choro /2
</commit_message>
<xml_diff>
--- a/La casa de papel.xlsx
+++ b/La casa de papel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arthu\Desktop\Documentos\Insper\2º_Periodo\Ciencia_dos_dados\twitter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C8F4A4B-9202-4308-8DAB-7DB0E42A0B75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A20F5612-5350-463D-BA42-D8E46235DA9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
@@ -2029,8 +2029,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B301"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A282" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A301" sqref="A301"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2092,7 +2092,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -2148,7 +2148,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -2172,7 +2172,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -2180,7 +2180,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -2196,7 +2196,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -2220,7 +2220,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
@@ -2228,7 +2228,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -2236,7 +2236,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -2252,7 +2252,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -2348,7 +2348,7 @@
         <v>38</v>
       </c>
       <c r="B39">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
@@ -2372,7 +2372,7 @@
         <v>41</v>
       </c>
       <c r="B42">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
@@ -2420,7 +2420,7 @@
         <v>47</v>
       </c>
       <c r="B48">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
@@ -2436,7 +2436,7 @@
         <v>49</v>
       </c>
       <c r="B50">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
@@ -2444,7 +2444,7 @@
         <v>50</v>
       </c>
       <c r="B51">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
@@ -2580,7 +2580,7 @@
         <v>67</v>
       </c>
       <c r="B68">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
@@ -2716,7 +2716,7 @@
         <v>84</v>
       </c>
       <c r="B85">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
@@ -2764,7 +2764,7 @@
         <v>90</v>
       </c>
       <c r="B91">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
@@ -2804,7 +2804,7 @@
         <v>95</v>
       </c>
       <c r="B96">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
@@ -2876,7 +2876,7 @@
         <v>104</v>
       </c>
       <c r="B105">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
@@ -2940,7 +2940,7 @@
         <v>112</v>
       </c>
       <c r="B113">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
@@ -2956,7 +2956,7 @@
         <v>114</v>
       </c>
       <c r="B115">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
@@ -3004,7 +3004,7 @@
         <v>120</v>
       </c>
       <c r="B121">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.3">
@@ -3020,7 +3020,7 @@
         <v>122</v>
       </c>
       <c r="B123">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.3">
@@ -3036,7 +3036,7 @@
         <v>124</v>
       </c>
       <c r="B125">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.3">
@@ -3228,7 +3228,7 @@
         <v>148</v>
       </c>
       <c r="B149">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.3">
@@ -3260,7 +3260,7 @@
         <v>152</v>
       </c>
       <c r="B153" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.3">
@@ -3372,7 +3372,7 @@
         <v>166</v>
       </c>
       <c r="B167" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.3">
@@ -3404,7 +3404,7 @@
         <v>170</v>
       </c>
       <c r="B171" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.3">
@@ -3500,7 +3500,7 @@
         <v>182</v>
       </c>
       <c r="B183" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.3">
@@ -3540,7 +3540,7 @@
         <v>187</v>
       </c>
       <c r="B188" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.3">
@@ -3556,7 +3556,7 @@
         <v>189</v>
       </c>
       <c r="B190" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.3">
@@ -3572,7 +3572,7 @@
         <v>191</v>
       </c>
       <c r="B192" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.3">
@@ -3692,7 +3692,7 @@
         <v>206</v>
       </c>
       <c r="B207" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.3">
@@ -3700,7 +3700,7 @@
         <v>207</v>
       </c>
       <c r="B208" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.3">
@@ -3756,7 +3756,7 @@
         <v>214</v>
       </c>
       <c r="B215" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.3">
@@ -3836,7 +3836,7 @@
         <v>224</v>
       </c>
       <c r="B225" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.3">
@@ -3876,7 +3876,7 @@
         <v>229</v>
       </c>
       <c r="B230" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.3">
@@ -3932,7 +3932,7 @@
         <v>236</v>
       </c>
       <c r="B237" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.3">
@@ -4092,7 +4092,7 @@
         <v>256</v>
       </c>
       <c r="B257" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.3">
@@ -4100,7 +4100,7 @@
         <v>257</v>
       </c>
       <c r="B258" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.3">
@@ -4132,7 +4132,7 @@
         <v>261</v>
       </c>
       <c r="B262" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.3">
@@ -4140,7 +4140,7 @@
         <v>262</v>
       </c>
       <c r="B263" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.3">
@@ -4188,7 +4188,7 @@
         <v>268</v>
       </c>
       <c r="B269" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.3">
@@ -4236,7 +4236,7 @@
         <v>274</v>
       </c>
       <c r="B275" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.3">
@@ -4316,7 +4316,7 @@
         <v>284</v>
       </c>
       <c r="B285" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.3">
@@ -4332,7 +4332,7 @@
         <v>286</v>
       </c>
       <c r="B287" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.3">
@@ -4340,7 +4340,7 @@
         <v>287</v>
       </c>
       <c r="B288" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.3">
@@ -4348,7 +4348,7 @@
         <v>288</v>
       </c>
       <c r="B289" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.3">
@@ -4364,7 +4364,7 @@
         <v>290</v>
       </c>
       <c r="B291" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.3">
@@ -4456,7 +4456,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A163" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A163" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="B203" sqref="B203"/>
     </sheetView>
   </sheetViews>

</xml_diff>